<commit_message>
Add quick and dirty version of the ST7xx library to work on MBED
</commit_message>
<xml_diff>
--- a/Documents/Arduino_GIGA_R1_pins.xlsx
+++ b/Documents/Arduino_GIGA_R1_pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Arduino_GIGA-stuff\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5921A16-D057-4993-BB37-A306D1514DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2E2298-DB2E-4C48-BA6E-DE7D40CBF371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="25890" windowHeight="17055" activeTab="3" xr2:uid="{4DF9CC89-F33A-471A-BC87-D2414FC11F80}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="25890" windowHeight="19215" firstSheet="1" activeTab="8" xr2:uid="{4DF9CC89-F33A-471A-BC87-D2414FC11F80}"/>
   </bookViews>
   <sheets>
     <sheet name="All Pins" sheetId="2" r:id="rId1"/>
@@ -40245,7 +40245,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:U169"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -68639,8 +68639,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68650,7 +68650,7 @@
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">

</xml_diff>